<commit_message>
6 sem start lab 6.11.1 nearly done
</commit_message>
<xml_diff>
--- a/4sem/452/tables/v2.xlsx
+++ b/4sem/452/tables/v2.xlsx
@@ -372,7 +372,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="K2" sqref="K2:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -381,978 +381,1181 @@
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>10</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
         <v>69</v>
-      </c>
-      <c r="C2" s="1">
-        <v>20</v>
       </c>
       <c r="D2" s="1">
         <v>20</v>
       </c>
       <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>1.2</v>
       </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
       <c r="I2" s="1">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
+      <c r="K2" s="1">
+        <f>J2*0.05+0.02</f>
+        <v>4.7500000000000001E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>14</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
         <v>49</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>28</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>20</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>12</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>0.27</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>0.6</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>0.97</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>0.45</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K33" si="0">J3*0.05+0.02</f>
+        <v>4.2500000000000003E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>16</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1">
         <v>62</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>28</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>20</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>24</v>
       </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>0.38</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <v>1.2</v>
       </c>
-      <c r="H4" s="1">
-        <v>1</v>
-      </c>
       <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
         <v>0.38</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>3.9000000000000007E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>18</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>76</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>42</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>24</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F5" s="1">
         <v>36</v>
       </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <v>1.5</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <v>0.98</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4500000000000003E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>20</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
         <v>69</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>39</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>24</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>35</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>1.5</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>0.98</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>0.28000000000000003</v>
       </c>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000002E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>22</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
         <v>55</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>42</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>35</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>0.13</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>2.5</v>
       </c>
-      <c r="H7" s="1">
+      <c r="I7" s="1">
         <v>0.9</v>
       </c>
-      <c r="I7" s="1">
+      <c r="J7" s="1">
         <v>0.15</v>
       </c>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>2.75E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>24</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
         <v>45</v>
       </c>
-      <c r="C8" s="1">
+      <c r="D8" s="1">
         <v>39</v>
       </c>
-      <c r="D8" s="1">
+      <c r="E8" s="1">
         <v>13</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>30</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="H8" s="1">
         <v>2.2999999999999998</v>
       </c>
-      <c r="H8" s="1">
+      <c r="I8" s="1">
         <v>0.92</v>
       </c>
-      <c r="I8" s="1">
+      <c r="J8" s="1">
         <v>0.08</v>
       </c>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="K8" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>26</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
         <v>46</v>
       </c>
-      <c r="C9" s="1">
+      <c r="D9" s="1">
         <v>38</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>8</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>33</v>
       </c>
-      <c r="F9" s="1">
+      <c r="G9" s="1">
         <v>0.1</v>
       </c>
-      <c r="G9" s="1">
+      <c r="H9" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H9" s="1">
+      <c r="I9" s="1">
         <v>0.79</v>
       </c>
-      <c r="I9" s="1">
+      <c r="J9" s="1">
         <v>0.12</v>
       </c>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="1">
+        <f t="shared" si="0"/>
+        <v>2.6000000000000002E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>28</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="1">
         <v>40</v>
       </c>
-      <c r="C10" s="1">
+      <c r="D10" s="1">
         <v>36</v>
       </c>
-      <c r="D10" s="1">
+      <c r="E10" s="1">
         <v>8</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>30</v>
       </c>
-      <c r="F10" s="1">
+      <c r="G10" s="1">
         <v>0.05</v>
       </c>
-      <c r="G10" s="1">
+      <c r="H10" s="1">
         <v>3.8</v>
       </c>
-      <c r="H10" s="1">
+      <c r="I10" s="1">
         <v>0.82</v>
       </c>
-      <c r="I10" s="1">
+      <c r="J10" s="1">
         <v>0.06</v>
       </c>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
+      <c r="K10" s="1">
+        <f t="shared" si="0"/>
+        <v>2.3E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>30</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
         <v>32</v>
       </c>
-      <c r="C11" s="1">
+      <c r="D11" s="1">
         <v>39</v>
       </c>
-      <c r="D11" s="1">
+      <c r="E11" s="1">
         <v>17</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>23</v>
       </c>
-      <c r="F11" s="1">
+      <c r="G11" s="1">
         <v>-0.1</v>
       </c>
-      <c r="G11" s="1">
+      <c r="H11" s="1">
         <v>1.4</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <v>0.99</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <v>0.1</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
+      <c r="K11" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>32</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1">
         <v>30</v>
       </c>
-      <c r="C12" s="1">
+      <c r="D12" s="1">
         <v>26</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>7</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>22</v>
       </c>
-      <c r="F12" s="1">
+      <c r="G12" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G12" s="1">
+      <c r="H12" s="1">
         <v>3.1</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <v>0.86</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <v>0.08</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>34</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
         <v>31</v>
       </c>
-      <c r="C13" s="1">
+      <c r="D13" s="1">
         <v>26</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>7</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>32</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="1">
         <v>0.09</v>
       </c>
-      <c r="G13" s="1">
+      <c r="H13" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <v>0.77</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <v>0.11</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="0"/>
+        <v>2.5500000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>38</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
         <v>40</v>
       </c>
-      <c r="C14" s="1">
+      <c r="D14" s="1">
         <v>36</v>
       </c>
-      <c r="D14" s="1">
+      <c r="E14" s="1">
         <v>7</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>30</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="1">
         <v>0.05</v>
       </c>
-      <c r="G14" s="1">
+      <c r="H14" s="1">
         <v>4.3</v>
       </c>
-      <c r="H14" s="1">
+      <c r="I14" s="1">
         <v>0.78</v>
       </c>
-      <c r="I14" s="1">
+      <c r="J14" s="1">
         <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="0"/>
+        <v>2.35E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>40</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
         <v>44</v>
       </c>
-      <c r="C15" s="1">
+      <c r="D15" s="1">
         <v>32</v>
       </c>
-      <c r="D15" s="1">
+      <c r="E15" s="1">
         <v>7</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>33</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="1">
         <v>0.16</v>
       </c>
-      <c r="G15" s="1">
+      <c r="H15" s="1">
         <v>4.7</v>
       </c>
-      <c r="H15" s="1">
+      <c r="I15" s="1">
         <v>0.76</v>
       </c>
-      <c r="I15" s="1">
+      <c r="J15" s="1">
         <v>0.21</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0499999999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>42</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
         <v>37</v>
       </c>
-      <c r="C16" s="1">
+      <c r="D16" s="1">
         <v>35</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>7</v>
       </c>
-      <c r="E16" s="1">
+      <c r="F16" s="1">
         <v>38</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="1">
         <v>0.03</v>
       </c>
-      <c r="G16" s="1">
+      <c r="H16" s="1">
         <v>5.4</v>
       </c>
-      <c r="H16" s="1">
+      <c r="I16" s="1">
         <v>0.72</v>
       </c>
-      <c r="I16" s="1">
+      <c r="J16" s="1">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K16" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>46</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
         <v>43</v>
       </c>
-      <c r="C17" s="1">
+      <c r="D17" s="1">
         <v>44</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>7</v>
       </c>
-      <c r="E17" s="1">
+      <c r="F17" s="1">
         <v>34</v>
       </c>
-      <c r="F17" s="1">
+      <c r="G17" s="1">
         <v>-0.01</v>
       </c>
-      <c r="G17" s="1">
+      <c r="H17" s="1">
         <v>4.9000000000000004</v>
       </c>
-      <c r="H17" s="1">
+      <c r="I17" s="1">
         <v>0.75</v>
       </c>
-      <c r="I17" s="1">
+      <c r="J17" s="1">
         <v>0.02</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K17" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>48</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
         <v>36</v>
       </c>
-      <c r="C18" s="1">
+      <c r="D18" s="1">
         <v>38</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>7</v>
       </c>
-      <c r="E18" s="1">
+      <c r="F18" s="1">
         <v>28</v>
       </c>
-      <c r="F18" s="1">
+      <c r="G18" s="1">
         <v>-0.03</v>
       </c>
-      <c r="G18" s="1">
+      <c r="H18" s="1">
         <v>4</v>
       </c>
-      <c r="H18" s="1">
+      <c r="I18" s="1">
         <v>0.8</v>
       </c>
-      <c r="I18" s="1">
+      <c r="J18" s="1">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K18" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>52</v>
       </c>
-      <c r="B19" s="1">
-        <v>52</v>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19" s="1">
         <v>52</v>
       </c>
       <c r="D19" s="1">
+        <v>52</v>
+      </c>
+      <c r="E19" s="1">
         <v>7</v>
       </c>
-      <c r="E19" s="1">
+      <c r="F19" s="1">
         <v>44</v>
       </c>
-      <c r="F19" s="1">
+      <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="1">
         <v>6.3</v>
       </c>
-      <c r="H19" s="1">
+      <c r="I19" s="1">
         <v>0.69</v>
       </c>
-      <c r="I19" s="1">
+      <c r="J19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>54</v>
       </c>
-      <c r="B20" s="1">
-        <v>48</v>
+      <c r="B20">
+        <v>1</v>
       </c>
       <c r="C20" s="1">
         <v>48</v>
       </c>
       <c r="D20" s="1">
+        <v>48</v>
+      </c>
+      <c r="E20" s="1">
         <v>7</v>
       </c>
-      <c r="E20" s="1">
+      <c r="F20" s="1">
         <v>39</v>
       </c>
-      <c r="F20" s="1">
+      <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="G20" s="1">
+      <c r="H20" s="1">
         <v>5.6</v>
       </c>
-      <c r="H20" s="1">
+      <c r="I20" s="1">
         <v>0.72</v>
       </c>
-      <c r="I20" s="1">
+      <c r="J20" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>56</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
         <v>46</v>
       </c>
-      <c r="C21" s="1">
+      <c r="D21" s="1">
         <v>44</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>7</v>
       </c>
-      <c r="E21" s="1">
+      <c r="F21" s="1">
         <v>38</v>
       </c>
-      <c r="F21" s="1">
+      <c r="G21" s="1">
         <v>0.02</v>
       </c>
-      <c r="G21" s="1">
+      <c r="H21" s="1">
         <v>5.4</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>0.72</v>
       </c>
-      <c r="I21" s="1">
+      <c r="J21" s="1">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K21" s="1">
+        <f t="shared" si="0"/>
+        <v>2.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>58</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
         <v>50</v>
       </c>
-      <c r="C22" s="1">
+      <c r="D22" s="1">
         <v>49</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>7</v>
       </c>
-      <c r="E22" s="1">
+      <c r="F22" s="1">
         <v>43</v>
       </c>
-      <c r="F22" s="1">
+      <c r="G22" s="1">
         <v>0.01</v>
       </c>
-      <c r="G22" s="1">
+      <c r="H22" s="1">
         <v>6.1</v>
       </c>
-      <c r="H22" s="1">
+      <c r="I22" s="1">
         <v>0.69</v>
       </c>
-      <c r="I22" s="1">
+      <c r="J22" s="1">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K22" s="1">
+        <f t="shared" si="0"/>
+        <v>2.0500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>60</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
         <v>58</v>
       </c>
-      <c r="C23" s="1">
+      <c r="D23" s="1">
         <v>51</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>19</v>
       </c>
-      <c r="E23" s="1">
+      <c r="F23" s="1">
         <v>37</v>
       </c>
-      <c r="F23" s="1">
+      <c r="G23" s="1">
         <v>0.06</v>
       </c>
-      <c r="G23" s="1">
+      <c r="H23" s="1">
         <v>1.9</v>
       </c>
-      <c r="H23" s="1">
+      <c r="I23" s="1">
         <v>0.95</v>
       </c>
-      <c r="I23" s="1">
+      <c r="J23" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K23" s="1">
+        <f t="shared" si="0"/>
+        <v>2.35E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>62</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
         <v>45</v>
       </c>
-      <c r="C24" s="1">
+      <c r="D24" s="1">
         <v>34</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>18</v>
       </c>
-      <c r="E24" s="1">
+      <c r="F24" s="1">
         <v>22</v>
       </c>
-      <c r="F24" s="1">
+      <c r="G24" s="1">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G24" s="1">
+      <c r="H24" s="1">
         <v>1.2</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>0.99</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K24" s="1">
+        <f t="shared" si="0"/>
+        <v>2.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>64</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
         <v>31</v>
       </c>
-      <c r="C25" s="1">
+      <c r="D25" s="1">
         <v>21</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>16</v>
       </c>
-      <c r="E25" s="1">
+      <c r="F25" s="1">
         <v>8</v>
       </c>
-      <c r="F25" s="1">
+      <c r="G25" s="1">
         <v>0.19</v>
       </c>
-      <c r="G25" s="1">
+      <c r="H25" s="1">
         <v>0.5</v>
       </c>
-      <c r="H25" s="1">
+      <c r="I25" s="1">
         <v>0.94</v>
       </c>
-      <c r="I25" s="1">
+      <c r="J25" s="1">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K25" s="1">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>66</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
         <v>62</v>
       </c>
-      <c r="C26" s="1">
+      <c r="D26" s="1">
         <v>34</v>
       </c>
-      <c r="D26" s="1">
+      <c r="E26" s="1">
         <v>16</v>
       </c>
-      <c r="E26" s="1">
+      <c r="F26" s="1">
         <v>32</v>
       </c>
-      <c r="F26" s="1">
+      <c r="G26" s="1">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G26" s="1">
+      <c r="H26" s="1">
         <v>2</v>
       </c>
-      <c r="H26" s="1">
+      <c r="I26" s="1">
         <v>0.94</v>
       </c>
-      <c r="I26" s="1">
+      <c r="J26" s="1">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K26" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>68</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
         <v>37</v>
       </c>
-      <c r="C27" s="1">
+      <c r="D27" s="1">
         <v>14</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E27" s="1">
         <v>16</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F27" s="1">
         <v>4</v>
       </c>
-      <c r="F27" s="1">
+      <c r="G27" s="1">
         <v>0.45</v>
       </c>
-      <c r="G27" s="1">
+      <c r="H27" s="1">
         <v>4</v>
       </c>
-      <c r="H27" s="1">
+      <c r="I27" s="1">
         <v>0.8</v>
       </c>
-      <c r="I27" s="1">
+      <c r="J27" s="1">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K27" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>70</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1">
         <v>60</v>
       </c>
-      <c r="C28" s="1">
+      <c r="D28" s="1">
         <v>24</v>
       </c>
-      <c r="D28" s="1">
+      <c r="E28" s="1">
         <v>16</v>
       </c>
-      <c r="E28" s="1">
+      <c r="F28" s="1">
         <v>20</v>
       </c>
-      <c r="F28" s="1">
+      <c r="G28" s="1">
         <v>0.43</v>
       </c>
-      <c r="G28" s="1">
+      <c r="H28" s="1">
         <v>1.3</v>
       </c>
-      <c r="H28" s="1">
+      <c r="I28" s="1">
         <v>0.99</v>
       </c>
-      <c r="I28" s="1">
+      <c r="J28" s="1">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K28" s="1">
+        <f t="shared" si="0"/>
+        <v>4.1500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>72</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1">
         <v>56</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29" s="1">
         <v>19</v>
       </c>
-      <c r="D29" s="1">
+      <c r="E29" s="1">
         <v>16</v>
       </c>
-      <c r="E29" s="1">
+      <c r="F29" s="1">
         <v>22</v>
       </c>
-      <c r="F29" s="1">
+      <c r="G29" s="1">
         <v>0.49</v>
       </c>
-      <c r="G29" s="1">
+      <c r="H29" s="1">
         <v>1.4</v>
       </c>
-      <c r="H29" s="1">
+      <c r="I29" s="1">
         <v>0.99</v>
       </c>
-      <c r="I29" s="1">
+      <c r="J29" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K29" s="1">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>74</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
         <v>43</v>
       </c>
-      <c r="C30" s="1">
+      <c r="D30" s="1">
         <v>14</v>
       </c>
-      <c r="D30" s="1">
+      <c r="E30" s="1">
         <v>10</v>
       </c>
-      <c r="E30" s="1">
+      <c r="F30" s="1">
         <v>19</v>
       </c>
-      <c r="F30" s="1">
+      <c r="G30" s="1">
         <v>0.51</v>
       </c>
-      <c r="G30" s="1">
+      <c r="H30" s="1">
         <v>1.9</v>
       </c>
-      <c r="H30" s="1">
+      <c r="I30" s="1">
         <v>0.95</v>
       </c>
-      <c r="I30" s="1">
+      <c r="J30" s="1">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K30" s="1">
+        <f t="shared" si="0"/>
+        <v>4.7E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>76</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
         <v>56</v>
       </c>
-      <c r="C31" s="1">
+      <c r="D31" s="1">
         <v>16</v>
       </c>
-      <c r="D31" s="1">
+      <c r="E31" s="1">
         <v>20</v>
       </c>
-      <c r="E31" s="1">
+      <c r="F31" s="1">
         <v>18</v>
       </c>
-      <c r="F31" s="1">
+      <c r="G31" s="1">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G31" s="1">
+      <c r="H31" s="1">
         <v>0.9</v>
       </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
       <c r="I31" s="1">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K31" s="1">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>78</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
         <v>52</v>
       </c>
-      <c r="C32" s="1">
+      <c r="D32" s="1">
         <v>19</v>
       </c>
-      <c r="D32" s="1">
+      <c r="E32" s="1">
         <v>21</v>
       </c>
-      <c r="E32" s="1">
+      <c r="F32" s="1">
         <v>14</v>
       </c>
-      <c r="F32" s="1">
+      <c r="G32" s="1">
         <v>0.46</v>
       </c>
-      <c r="G32" s="1">
+      <c r="H32" s="1">
         <v>0.7</v>
       </c>
-      <c r="H32" s="1">
+      <c r="I32" s="1">
         <v>0.98</v>
       </c>
-      <c r="I32" s="1">
+      <c r="J32" s="1">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K32" s="1">
+        <f t="shared" si="0"/>
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>80</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
         <v>41</v>
       </c>
-      <c r="C33" s="1">
+      <c r="D33" s="1">
         <v>18</v>
       </c>
-      <c r="D33" s="1">
+      <c r="E33" s="1">
         <v>20</v>
       </c>
-      <c r="E33" s="1">
+      <c r="F33" s="1">
         <v>10</v>
       </c>
-      <c r="F33" s="1">
+      <c r="G33" s="1">
         <v>0.39</v>
       </c>
-      <c r="G33" s="1">
+      <c r="H33" s="1">
         <v>0.5</v>
       </c>
-      <c r="H33" s="1">
+      <c r="I33" s="1">
         <v>0.94</v>
       </c>
-      <c r="I33" s="1">
+      <c r="J33" s="1">
         <v>0.41</v>
+      </c>
+      <c r="K33" s="1">
+        <f t="shared" si="0"/>
+        <v>4.0500000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>